<commit_message>
add: 추가 google-lint, 추가 docker-DB manual
</commit_message>
<xml_diff>
--- a/Document/기술 문서/rest_api.xlsx
+++ b/Document/기술 문서/rest_api.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SSAFY\B104\S10P12B104\Document\기술 문서\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SSAFY\VSCODE\goodeyedeer\back\S10P12B104\Document\기술 문서\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <t>회원</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -792,6 +792,36 @@
 {
  변경사항
 }</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 탈퇴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DELETE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> user</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -956,7 +986,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1022,6 +1052,9 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1355,10 +1388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:H12"/>
+  <dimension ref="C1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1392,7 +1425,7 @@
       </c>
     </row>
     <row r="2" spans="3:8" ht="18" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="23" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="10" t="s">
@@ -1406,7 +1439,7 @@
       <c r="H2" s="13"/>
     </row>
     <row r="3" spans="3:8" x14ac:dyDescent="0.4">
-      <c r="C3" s="23"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1418,7 +1451,7 @@
       <c r="H3" s="14"/>
     </row>
     <row r="4" spans="3:8" ht="365.4" x14ac:dyDescent="0.4">
-      <c r="C4" s="23"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1434,7 +1467,7 @@
       <c r="H4" s="15"/>
     </row>
     <row r="5" spans="3:8" ht="104.4" x14ac:dyDescent="0.4">
-      <c r="C5" s="23"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1450,8 +1483,8 @@
       <c r="H5" s="14"/>
     </row>
     <row r="6" spans="3:8" ht="104.4" x14ac:dyDescent="0.4">
-      <c r="C6" s="23"/>
-      <c r="D6" s="1" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="22" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -1465,50 +1498,50 @@
       </c>
       <c r="H6" s="14"/>
     </row>
-    <row r="7" spans="3:8" ht="409.6" x14ac:dyDescent="0.4">
-      <c r="C7" s="24" t="s">
+    <row r="7" spans="3:8" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="C7" s="24"/>
+      <c r="D7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="14"/>
+    </row>
+    <row r="8" spans="3:8" ht="409.6" x14ac:dyDescent="0.4">
+      <c r="C8" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="H7" s="16"/>
-    </row>
-    <row r="8" spans="3:8" ht="156.6" x14ac:dyDescent="0.4">
-      <c r="C8" s="25"/>
-      <c r="D8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="H8" s="16"/>
     </row>
-    <row r="9" spans="3:8" ht="69.599999999999994" x14ac:dyDescent="0.4">
-      <c r="C9" s="25"/>
+    <row r="9" spans="3:8" ht="156.6" x14ac:dyDescent="0.4">
+      <c r="C9" s="26"/>
       <c r="D9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>30</v>
+        <v>24</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>28</v>
@@ -1516,60 +1549,76 @@
       <c r="H9" s="16"/>
     </row>
     <row r="10" spans="3:8" ht="69.599999999999994" x14ac:dyDescent="0.4">
-      <c r="C10" s="25"/>
-      <c r="D10" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>42</v>
+      <c r="C10" s="26"/>
+      <c r="D10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="17"/>
+      <c r="H10" s="16"/>
     </row>
-    <row r="11" spans="3:8" ht="174" x14ac:dyDescent="0.4">
-      <c r="C11" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>40</v>
+    <row r="11" spans="3:8" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="C11" s="26"/>
+      <c r="D11" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="18"/>
+      <c r="H11" s="17"/>
     </row>
-    <row r="12" spans="3:8" ht="226.2" x14ac:dyDescent="0.4">
-      <c r="C12" s="27"/>
+    <row r="12" spans="3:8" ht="174" x14ac:dyDescent="0.4">
+      <c r="C12" s="27" t="s">
+        <v>26</v>
+      </c>
       <c r="D12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="19"/>
+      <c r="H12" s="18"/>
+    </row>
+    <row r="13" spans="3:8" ht="226.2" x14ac:dyDescent="0.4">
+      <c r="C13" s="28"/>
+      <c r="D13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Docs: 수정 ERD 및 API 명세서
</commit_message>
<xml_diff>
--- a/Document/기술 문서/rest_api.xlsx
+++ b/Document/기술 문서/rest_api.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>회원</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -108,76 +108,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">get user  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>//전체 회원 (관리자 사용)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-get user?role=0 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">//admin 회원 조회
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-get user?email=test@gmail.com  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>//email=test@gmail.com</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>QueryDSL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>프로필 이미지 수정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -215,74 +145,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>post user/nickname
-{
- userId: 'id'
- accessToken: 'Token'
- nickname: 'hong'
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">200
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[
-  {
-    id:3,
-    role:0
-    user_name:'honggildong'
-    nickname:'banana'
-    profile_image:'user/image/123.jpg',
-    provider : google
-    accessToken: abc
-  },
-  {
-    id:1,
-    role:1
-    user_name:'yepo'
-    nickname:'nike'
-    profile_image:'user/image/334.jpg'
-    provider : google
-    accessToken: abc
-  }
-]</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">post user/profile_img 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{
- userId: 'id'
- accessToken: 'Token'
- image: 'img url'
-}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>프로젝트</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -291,143 +153,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>get project</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> // 전체 프로젝트 (관리자 사용)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">get project?user='user' </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>// user 프로젝트 검색</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>200</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-[
-  {
-    projectId: 3,
-    projectName: 'Name'
-    templateId: 1
-    projectUpdateTime: YYYY-MM-DD
-    contributor: {
-     user1
-     user2
-    }
-    chatLog: {
-     chat
-    }
-    children: {
-     content
-    }
-  },
-  {
-    projectId: 4,
-    projectName: 'Name'
-    templateId: 1
-    projectUpdateTime: YYYY-MM-DD
-    contributor: {
-     user1
-     user2
-    }
-    chatLog: {
-     chat
-    }
-    children: {
-     content
-    }
-  }
-]</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>프로젝트 요약 검색</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">get project/summary?user='user' </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>// user 프로젝트 요약 검색</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -666,117 +392,6 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">get template/info?templateId=1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>// 템플릿 내용 호출</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>200</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-[
- {
-  projectId: 1
-  projectName: 'Name'
-  projectUpdateTime: YYYY-MM-DD
-  thumbnail: 'URL'
- }
-]</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>200</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-[
- {
-  templatetId: 1
-  templateName: 'Name'
-  templateUpdateTime: YYYY-MM-DD
-  templateAuthor: 'Author'
-  thumbnail: 'URL'
- }
-]</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>200
-[
- {
-  templatetId: 1
-  templateName: 'Name'
-  templateUpdateTime: YYYY-MM-DD
-  templateAuthor: 'Author'
-  thumbnail: 'URL'
-  children {
-    childrenInfo
-  }
- }
-]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>patch workList</t>
     </r>
     <r>
@@ -810,6 +425,205 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
+      <t>200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+{
+    "projectId" : "pjt1",
+    "templateId" : "template1",
+    "projectName" : "PJT_NAME",
+    "updateTime" : "2024-01-01",
+    "thumbnail" : "imageUrl",
+    "locationIds" : [
+        "lId1",
+        "lId2",
+        "lId3"
+    ],
+    "chatLog" : [
+        {
+            "name" : "userName1",
+            "profile" : "userProfile1",
+            "time" : "2024-01-01T00:00:00",
+            "content" : "chat1"
+        },
+        {
+            "name" : "userName2",
+            "profile" : "userProfile2",
+            "time" : "2024-01-01T00:00:00",
+            "content" : "chat2"
+        },
+        {
+            "name" : "userName3",
+            "profile" : "userProfile3",
+            "time" : "2024-01-01T00:00:00",
+            "content" : "chat3"
+        }
+    ],
+    "children" : [
+        {
+            "id" : "Rect1",
+            "type" : "Rect",
+            "x" : 0,
+            "y" : 0,
+            "width" : 0,
+            "height" : 0,
+            "fill" : "#FFFFFF",
+            "stroke" : "#FFFFFF",
+            "strokeWidth" : 1,
+            "rotation" : 0,
+            "opacity" : 0,
+            "visible" : false,
+            "draggable" : false
+        },
+        {
+            "id" : "Circle1",
+            "type" : "Circle",
+            "x" : 0,
+            "y" : 0,
+            "radius" : 0,
+            "fill" : "#FFFFFF",
+            "stroke" : "#FFFFFF",
+            "strokeWidth" : 1,
+            "rotation" : 0,
+            "opacity" : 0,
+            "visible" : false,
+            "draggable" : false
+        },
+        {
+            "id" : "ReqularPolygon1",
+            "type" : "ReqularPolygon",
+            "x" : 0,
+            "y" : 0,
+            "sides" : 3,
+            "radius" : 0,
+            "fill" : "#FFFFFF",
+            "stroke" : "#FFFFFF",
+            "strokeWidth" : 1,
+            "rotation" : 0,
+            "opacity" : 0,
+            "visible" : false,
+            "draggable" : false
+        },
+        {
+            "id" : "Line1",
+            "type" : "Line",
+            "points": [0, 0, 100, 100],
+            "stroke": "#000000",
+            "strokeWidth": 2,
+            "lineCap": "round",
+            "lineJoin": "bevel",
+            "dash": [5, 5],
+            "rotation": 0,
+            "opacity": 1.0,
+            "visible": true,
+            "draggable": true
+        },
+        {
+            "id" : "Text1",
+            "type" : "Text",
+            "x": 0,
+            "y": 0,
+            "text": "textContent",
+            "fontSize": 12,
+            "fontFamily": "Arial",
+            "fill": "#000000",
+            "stroke": "#FFFFFF",
+            "strokeWidth": 1,
+            "rotation": 0,
+            "opacity": 1.0,
+            "visible": true,
+            "draggable": true
+        },
+        {
+            "id" : "Arrow1",
+            "type" : "Arrow",
+            "points": [0, 0, 100, 100],
+            "pointerLength": 10,
+            "pointerWidth": 10,
+            "fill": "#000000",
+            "stroke": "#000000",
+            "strokeWidth": 2,
+            "rotation": 0,
+            "opacity": 1.0,
+            "visible": true,
+            "draggable": true
+          }
+    ]
+}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+{
+ msg: 'success'
+}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">post user/profile_img 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{
+ "userId": INTEGER
+ "accessToken": 'Token'
+ "image": 'img url'
+}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>DELETE</t>
     </r>
     <r>
@@ -821,7 +635,530 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> user</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>user?id=2</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>get project</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> // 전체 프로젝트 (관리자 사용)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">get project?userId=1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">// user 프로젝트 검색
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>get project?userId=1&amp;folderId=1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> // user의 폴더 내 프로젝트 검색</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">get project/summary?userId=1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">// user 프로젝트 요약 검색
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">get project/summary?userId=1&amp;folderId=1 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>// user의 폴더 내 프로젝트 요약 검색</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+[
+ {
+  "projectId": "pjt1"
+  "projectName": 'Name1'
+  "projectUpdateTime": YYYY-MM-DDTHH:MM:SS
+  "thumbnail": 'URL'
+ },
+{
+  "projectId": "pjt2"
+  "projectName": 'Name2'
+  "projectUpdateTime": YYYY-MM-DDTHH:MM:SS
+  "thumbnail": 'URL'
+ }
+]</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>post user/nickname</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+{
+ "userId": INTEGER
+ "accessToken": 'Token'
+ "nickname": 'hong'
+}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">200
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{
+    "templateId" : "template1",
+    "templateName" : "tmp_NAME",
+    "templatePrice" : 0,
+    "templateAuthor" : "admin",
+    "templateUpdateTime" : "2024-01-01",
+    "thumbnail" : "imageUrl",
+    "description" : "template_description",
+    "children" : [
+        {
+            "id" : "Rect1",
+            "type" : "Rect",
+            "x" : 0,
+            "y" : 0,
+            "width" : 0,
+            "height" : 0,
+            "fill" : "#FFFFFF",
+            "stroke" : "#FFFFFF",
+            "strokeWidth" : 1,
+            "rotation" : 0,
+            "opacity" : 0,
+            "visible" : false,
+            "draggable" : false
+        },
+        {
+            "id" : "Circle1",
+            "type" : "Circle",
+            "x" : 0,
+            "y" : 0,
+            "radius" : 0,
+            "fill" : "#FFFFFF",
+            "stroke" : "#FFFFFF",
+            "strokeWidth" : 1,
+            "rotation" : 0,
+            "opacity" : 0,
+            "visible" : false,
+            "draggable" : false
+        },
+        {
+            "id" : "ReqularPolygon1",
+            "type" : "ReqularPolygon",
+            "x" : 0,
+            "y" : 0,
+            "sides" : 3,
+            "radius" : 0,
+            "fill" : "#FFFFFF",
+            "stroke" : "#FFFFFF",
+            "strokeWidth" : 1,
+            "rotation" : 0,
+            "opacity" : 0,
+            "visible" : false,
+            "draggable" : false
+        },
+        {
+            "id" : "Line1",
+            "type" : "Line",
+            "points": [0, 0, 100, 100],
+            "stroke": "#000000",
+            "strokeWidth": 2,
+            "lineCap": "round",
+            "lineJoin": "bevel",
+            "dash": [5, 5],
+            "rotation": 0,
+            "opacity": 1.0,
+            "visible": true,
+            "draggable": true
+        },
+        {
+            "id" : "Text1",
+            "type" : "Text",
+            "x": 0,
+            "y": 0,
+            "text": "textContent",
+            "fontSize": 12,
+            "fontFamily": "Arial",
+            "fill": "#000000",
+            "stroke": "#FFFFFF",
+            "strokeWidth": 1,
+            "rotation": 0,
+            "opacity": 1.0,
+            "visible": true,
+            "draggable": true
+        },
+        {
+            "id" : "Arrow1",
+            "type" : "Arrow",
+            "points": [0, 0, 100, 100],
+            "pointerLength": 10,
+            "pointerWidth": 10,
+            "fill": "#000000",
+            "stroke": "#000000",
+            "strokeWidth": 2,
+            "rotation": 0,
+            "opacity": 1.0,
+            "visible": true,
+            "draggable": true
+          }
+    ]
+}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>200
+[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ {
+   "templatetId": 1,
+   "templateName": 'Name',
+   "templateUpdateTime": "2024-01-01" ,
+   "templateAuthor": 'Author',
+   "description" : "template_description"
+   "thumbnail": 'URL',
+ },
+...
+]</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">get template/info?templateId="template1" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>// 템플릿 내용 호출</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">200
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[
+  {
+    "userId": 0,
+    "email": "test@gmail.com",
+    "isAdmin":0,
+    "userName":'honggildong',
+    "profileImg":'user/image/123.jpg',
+    "provider" : 'google',
+    "accessToken": 'abc'
+  },
+  {
+    "userId": 1,
+    "email": "other@gmail.com"
+    "isAdmin":1,
+    "userName":'yepo',
+    "profileImg":'user/image/334.jpg'
+    "provider": 'google',
+    accessToken: 'abc'
+  }
+]</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">get user  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//전체 회원 (관리자 사용)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+get user?isAdmin=0 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">//admin 조회
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+get user?email="test@gmail.com"  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">//email=test@gmail.com
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">get user?id=1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>// id로 회원 조회</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1390,8 +1727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1420,9 +1757,7 @@
       <c r="G1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>13</v>
-      </c>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="3:8" ht="18" thickTop="1" x14ac:dyDescent="0.4">
       <c r="C2" s="23" t="s">
@@ -1456,10 +1791,10 @@
         <v>8</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>9</v>
@@ -1469,148 +1804,148 @@
     <row r="5" spans="3:8" ht="104.4" x14ac:dyDescent="0.4">
       <c r="C5" s="24"/>
       <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="H5" s="14"/>
     </row>
     <row r="6" spans="3:8" ht="104.4" x14ac:dyDescent="0.4">
       <c r="C6" s="24"/>
       <c r="D6" s="22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H6" s="14"/>
     </row>
     <row r="7" spans="3:8" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="C7" s="24"/>
       <c r="D7" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="3:8" ht="409.6" x14ac:dyDescent="0.4">
+    <row r="8" spans="3:8" ht="408.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C8" s="25" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="F8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="H8" s="16"/>
     </row>
-    <row r="9" spans="3:8" ht="156.6" x14ac:dyDescent="0.4">
+    <row r="9" spans="3:8" ht="295.8" x14ac:dyDescent="0.4">
       <c r="C9" s="26"/>
       <c r="D9" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H9" s="16"/>
     </row>
     <row r="10" spans="3:8" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="C10" s="26"/>
       <c r="D10" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H10" s="16"/>
     </row>
     <row r="11" spans="3:8" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="C11" s="26"/>
       <c r="D11" s="17" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H11" s="17"/>
     </row>
-    <row r="12" spans="3:8" ht="174" x14ac:dyDescent="0.4">
+    <row r="12" spans="3:8" ht="208.8" x14ac:dyDescent="0.4">
       <c r="C12" s="27" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>28</v>
+        <v>41</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="H12" s="18"/>
     </row>
-    <row r="13" spans="3:8" ht="226.2" x14ac:dyDescent="0.4">
+    <row r="13" spans="3:8" ht="409.6" x14ac:dyDescent="0.4">
       <c r="C13" s="28"/>
       <c r="D13" s="4" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>28</v>
+        <v>40</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="H13" s="19"/>
     </row>

</xml_diff>